<commit_message>
Added a data structures section
</commit_message>
<xml_diff>
--- a/Prep.xlsx
+++ b/Prep.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1131965\Documents\VSCode\AWSPrep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1131965\Documents\VSCode\AWSPrep\coding_prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5715B145-413E-4259-B4F8-46B7F39FC1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D71CF-F67D-4929-ADCE-9591C1C6CE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39765" yWindow="4935" windowWidth="23550" windowHeight="6000" xr2:uid="{B0CD7087-9F3A-4754-A4C4-AEA763DF9BEC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B0CD7087-9F3A-4754-A4C4-AEA763DF9BEC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sorting Algorithms" sheetId="1" r:id="rId1"/>
-    <sheet name="BST" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Structures" sheetId="3" r:id="rId1"/>
+    <sheet name="Sorting Algorithms" sheetId="1" r:id="rId2"/>
+    <sheet name="BST" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Traversals:</t>
   </si>
@@ -107,6 +108,92 @@
     Shift left_element to the right
     Decrease left index by 1
 Else store tobe_sorted at left_index + 1</t>
+  </si>
+  <si>
+    <t>Array/List</t>
+  </si>
+  <si>
+    <t>Contiguous sreial data</t>
+  </si>
+  <si>
+    <t>Pros</t>
+  </si>
+  <si>
+    <t>Cons</t>
+  </si>
+  <si>
+    <t>Efficient search when data is ordered</t>
+  </si>
+  <si>
+    <t>Inefficient insert and delete since data needs to be shifted</t>
+  </si>
+  <si>
+    <t>Hash table</t>
+  </si>
+  <si>
+    <t>table of key values</t>
+  </si>
+  <si>
+    <t>Fast for search, insert and delete</t>
+  </si>
+  <si>
+    <t>Unordered data</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Data ordered in LIFO</t>
+  </si>
+  <si>
+    <t>Data ordered in FIFO</t>
+  </si>
+  <si>
+    <t>Efficient access operations</t>
+  </si>
+  <si>
+    <t>Can only acces the top of the stack</t>
+  </si>
+  <si>
+    <t>Can only access the front of the queue</t>
+  </si>
+  <si>
+    <t>Linked list</t>
+  </si>
+  <si>
+    <t>Similar to an array but
+spread across different memory areas</t>
+  </si>
+  <si>
+    <t>No need to shift data upon 
+insert and delete</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Node based data structure.
+Each tree has a root with 0 or more children. Can't contain cycles</t>
+  </si>
+  <si>
+    <t>Data is 
+scattered in random memory locations</t>
+  </si>
+  <si>
+    <t>Fast for search, insert and delete.
+Ordered data.</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Node based data structure, data doesn not need to be organized and can have cycles</t>
+  </si>
+  <si>
+    <t>Good fit for relational data</t>
   </si>
 </sst>
 </file>
@@ -476,22 +563,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268DB3C0-AD4D-4D5B-B725-A35335D310F4}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD845997-ABAC-45DD-91C3-97C9F376A19C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -506,7 +720,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -520,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -539,7 +753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC09EA4-7477-40ED-89BC-C59387BCFC31}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -547,21 +761,21 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -572,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -583,7 +797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -597,7 +811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -635,7 +849,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD451492-5D04-4662-B724-501D7A201619}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{760AA9E2-CE56-4300-A915-6055CFAF40A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>